<commit_message>
Updated meeting tracker with today's minutes
</commit_message>
<xml_diff>
--- a/SE_4351.001_Group_3_Meeting_Tracker.xlsx
+++ b/SE_4351.001_Group_3_Meeting_Tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\salty\Documents\School\SE 4351\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3588E0B-7181-4853-B84F-EF791E4BC9DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02D04146-0F20-4B31-A7F9-32860140E11D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MeetingTracker" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="50">
   <si>
     <t>Meeting Date</t>
   </si>
@@ -149,6 +149,48 @@
   </si>
   <si>
     <t>Complete your slides for your portion of the presentation</t>
+  </si>
+  <si>
+    <t>Rayan B. Ashlee K. Micheal K. Michael U.</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Business Events\Use Cases</t>
+  </si>
+  <si>
+    <t>Initial Feature Set</t>
+  </si>
+  <si>
+    <t>Feb 6th</t>
+  </si>
+  <si>
+    <t>Independently brainstorm as many events and use cases as you can. Document them all somehow (pdf, docx, etc).</t>
+  </si>
+  <si>
+    <t>Independently brainstorm as many features as you can. Document them all somehow (pdf, docx, etc).</t>
+  </si>
+  <si>
+    <t>Additional Notes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The following deliverables were not at delivered at the meeting. They must be delivered to PM by 5:00 pm today January 30th, 2023. Any deliverables received after that time will not be included in the assignment submission. This is to give the PM time to review and assemble the deliverables for submission to Dr. Smith at 9:00am on January 31st, 2023. </t>
+  </si>
+  <si>
+    <t>Deliverables for assignment 1 discussed. Assignment 2 instructions were reviewed. Each member will independently brainstorm as many business events, business use cases, and initial features as they could and bring them to the next meeting</t>
+  </si>
+  <si>
+    <t>Bio information and photo - Rayan B, Ashlee K
+Presentation slides - Rayan B, Ashlee K, Michael U
+Introduction video - Rayan B, Ashlee K, Michael U
+Presentation video - Rayan B, Ashlee K, Michael U
+Work context diagram - Rayan B
+Stakeholder mapping - Ashlee K
+Team Bio - Michael U (Blocker: Need info and photos from Rayan B and Ashlee K)</t>
   </si>
 </sst>
 </file>
@@ -186,7 +228,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -225,13 +267,73 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="thin">
+      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
@@ -249,9 +351,7 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -264,9 +364,7 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -279,162 +377,186 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -716,203 +838,272 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.42578125" customWidth="1"/>
-    <col min="2" max="2" width="37.140625" customWidth="1"/>
+    <col min="2" max="2" width="40.5703125" customWidth="1"/>
     <col min="3" max="3" width="22.140625" customWidth="1"/>
     <col min="4" max="4" width="52.28515625" customWidth="1"/>
+    <col min="5" max="5" width="39.42578125" customWidth="1"/>
+    <col min="6" max="6" width="53.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="30" t="s">
         <v>12</v>
       </c>
       <c r="B1" s="30"/>
-      <c r="C1" s="30" t="s">
+      <c r="C1" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="30"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="33"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="23"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="33"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="27" t="s">
+      <c r="C3" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="28" t="s">
+      <c r="D3" s="34" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="29">
+      <c r="E3" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="F3" s="16"/>
+    </row>
+    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="15">
         <v>44949</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="35" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="6"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="2"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="1"/>
+    </row>
+    <row r="5" spans="1:6" ht="149.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="22">
+        <v>44956</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="39" t="s">
+        <v>48</v>
+      </c>
+      <c r="E5" s="38" t="s">
+        <v>47</v>
+      </c>
+      <c r="F5" s="40" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="4"/>
       <c r="B6" s="1"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="2"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="6"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="2"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="4"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="35"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="4"/>
       <c r="B8" s="1"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="2"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="35"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="4"/>
       <c r="B9" s="1"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="2"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="35"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="4"/>
       <c r="B10" s="1"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="2"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="35"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="4"/>
       <c r="B11" s="1"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="2"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="35"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="4"/>
       <c r="B12" s="1"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="2"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="35"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="4"/>
       <c r="B13" s="1"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="2"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="35"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="4"/>
       <c r="B14" s="1"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="2"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="35"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="4"/>
       <c r="B15" s="1"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="2"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="35"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="4"/>
       <c r="B16" s="1"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="2"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="35"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="4"/>
       <c r="B17" s="1"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="2"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="35"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="4"/>
       <c r="B18" s="1"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="2"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="35"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="4"/>
       <c r="B19" s="1"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="2"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="35"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="4"/>
       <c r="B20" s="1"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="2"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="35"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="4"/>
       <c r="B21" s="1"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="2"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="35"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="4"/>
       <c r="B22" s="1"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="2"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="35"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="4"/>
       <c r="B23" s="1"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="2"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="35"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="4"/>
       <c r="B24" s="1"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="2"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="6"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="35"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="4"/>
       <c r="B25" s="1"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="2"/>
-    </row>
-    <row r="26" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="7"/>
-      <c r="B26" s="3"/>
-      <c r="C26" s="9"/>
-      <c r="D26" s="4"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="35"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+    </row>
+    <row r="26" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="5"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="36"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="C1:F1"/>
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="A2:D2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -921,224 +1112,271 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42AE390D-D924-4FC4-ABD3-49EB24E8C851}">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.5703125" customWidth="1"/>
     <col min="3" max="3" width="14.28515625" customWidth="1"/>
     <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="51.7109375" customWidth="1"/>
+    <col min="5" max="5" width="18.140625" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" customWidth="1"/>
+    <col min="7" max="7" width="61.42578125" style="29" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="19" t="s">
+      <c r="B1" s="18"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="20"/>
+      <c r="G1" s="19"/>
     </row>
     <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="16"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="27"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="13" t="s">
+      <c r="G3" s="28" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="8">
+      <c r="A4" s="6">
         <v>1</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F4" s="17" t="s">
+      <c r="F4" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="6">
+        <v>1</v>
+      </c>
+      <c r="B5" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G4" s="5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="8">
+      <c r="G5" s="3"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="6">
         <v>1</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" s="5" t="s">
+      <c r="B6" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E6" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F5" s="17" t="s">
+      <c r="F6" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G5" s="1"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="8">
+      <c r="G6" s="3"/>
+    </row>
+    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="6">
         <v>1</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" s="5" t="s">
+      <c r="B7" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E7" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F6" s="17" t="s">
+      <c r="F7" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G6" s="1"/>
-    </row>
-    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="8">
+      <c r="G7" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="6">
         <v>1</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" s="5" t="s">
+      <c r="B8" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E8" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="F7" s="17" t="s">
+      <c r="F8" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="G7" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="8">
+      <c r="G8" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="6">
         <v>1</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C8" s="1" t="s">
+      <c r="B9" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D9" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E9" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="F8" s="8" t="s">
+      <c r="F9" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="G8" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="8">
+      <c r="G9" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="6">
         <v>1</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C9" s="1" t="s">
+      <c r="B10" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D10" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E10" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="F9" s="8" t="s">
+      <c r="F10" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="G9" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="8">
-        <v>1</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C10" s="1" t="s">
+      <c r="G10" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="23">
+        <v>2</v>
+      </c>
+      <c r="B11" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="D10" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E10" s="1" t="s">
+      <c r="D11" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="F10" s="8" t="s">
+      <c r="E11" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="F11" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="G10" s="5" t="s">
-        <v>37</v>
+      <c r="G11" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="23">
+        <v>2</v>
+      </c>
+      <c r="B12" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="F12" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>